<commit_message>
Configure for Render deployment with persistent databases
- Add Render-compatible Dockerfile with persistent /data volume support
  * Multi-stage build: Maven builder + lightweight JRE runtime
  * Initialization script handles first-run database setup
  * Subsequent runs use databases from persistent disk

- Update DatabaseUtil.java to check for Render's /data mount point
  * First checks /data (Render persistent disk)
  * Falls back to local development directory structure
  * Seamless environment detection

- Simplify application.properties
  * Remove unused H2 datasource configuration
  * Disable Spring Boot DataSource auto-configuration
  * Keep session persistence settings for user authentication

- Remove test enforcement plugin from pom.xml
  * Allows Docker builds to skip tests with -DskipTests
  * Faster builds without breaking test infrastructure
</commit_message>
<xml_diff>
--- a/navisewebsite/src/main/java/com/example/navisewebsite/repository/courses.xlsx
+++ b/navisewebsite/src/main/java/com/example/navisewebsite/repository/courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nsm2004/Desktop/Tulane/SoftwareStudio/Navise-CMPS-3300---Software-Studio-F25/navisewebsite/src/main/java/com/example/navisewebsite/repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E07F9-BB99-A847-A7B6-0B3A098856A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA01975-83B1-E746-A02A-13F491495E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{7C8C3A7A-5DDD-1C47-8967-F889625D71CC}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20480" activeTab="3" xr2:uid="{7C8C3A7A-5DDD-1C47-8967-F889625D71CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Computer Science" sheetId="1" r:id="rId1"/>
@@ -1984,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F42229-1492-4E4F-A408-388A98174DED}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B28" sqref="B28"/>
     </sheetView>
@@ -2837,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBFA97F-806E-41BE-B331-5EA3BA182B73}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>